<commit_message>
Hafta 8 veri modeli ve raporu oluşturuldu
</commit_message>
<xml_diff>
--- a/Seferihisar.xlsx
+++ b/Seferihisar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\4. Sınıf\Yazılım Müh. Günc. Konular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\4. Sınıf\Yazılım Müh. Günc. Konular\YmgkProject\havakalite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -422,10 +422,10 @@
   <dimension ref="A1:I1418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E825" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="J839" sqref="J839"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24727,6 +24727,9 @@
       <c r="H839">
         <v>19.65287</v>
       </c>
+      <c r="I839">
+        <v>10.314987</v>
+      </c>
     </row>
     <row r="840" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A840" s="2">

</xml_diff>